<commit_message>
dashboard completo  y  informe pdf corregido
</commit_message>
<xml_diff>
--- a/app/static/inventario_calculado.xlsx
+++ b/app/static/inventario_calculado.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q14"/>
+  <dimension ref="A1:S14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -500,25 +500,35 @@
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
+          <t>Unnamed: 12</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 13</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
           <t>Demanda diaria</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Stock mínimo</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Stock seguridad</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Stock máximo</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Mes</t>
         </is>
@@ -559,25 +569,27 @@
       <c r="J2" t="n">
         <v>800000</v>
       </c>
-      <c r="K2" t="n">
-        <v>900000</v>
-      </c>
+      <c r="K2" t="inlineStr"/>
       <c r="L2" s="2" t="n">
         <v>45879</v>
       </c>
-      <c r="M2" t="n">
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="n">
+        <v>2840000</v>
+      </c>
+      <c r="O2" t="n">
         <v>2</v>
       </c>
-      <c r="N2" t="n">
+      <c r="P2" t="n">
         <v>10</v>
       </c>
-      <c r="O2" t="n">
+      <c r="Q2" t="n">
         <v>0.5</v>
       </c>
-      <c r="P2" t="n">
+      <c r="R2" t="n">
         <v>10.5</v>
       </c>
-      <c r="Q2" t="inlineStr">
+      <c r="S2" t="inlineStr">
         <is>
           <t>August 2025</t>
         </is>
@@ -618,25 +630,25 @@
       <c r="J3" t="n">
         <v>900000</v>
       </c>
-      <c r="K3" t="n">
-        <v>300000</v>
-      </c>
+      <c r="K3" t="inlineStr"/>
       <c r="L3" s="2" t="n">
         <v>45880</v>
       </c>
-      <c r="M3" t="n">
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="n">
         <v>2.666666666666667</v>
       </c>
-      <c r="N3" t="n">
+      <c r="P3" t="n">
         <v>18.66666666666666</v>
       </c>
-      <c r="O3" t="n">
+      <c r="Q3" t="n">
         <v>0.9333333333333332</v>
       </c>
-      <c r="P3" t="n">
+      <c r="R3" t="n">
         <v>19.6</v>
       </c>
-      <c r="Q3" t="inlineStr">
+      <c r="S3" t="inlineStr">
         <is>
           <t>August 2025</t>
         </is>
@@ -677,25 +689,25 @@
       <c r="J4" t="n">
         <v>150000</v>
       </c>
-      <c r="K4" t="n">
-        <v>100000</v>
-      </c>
+      <c r="K4" t="inlineStr"/>
       <c r="L4" s="2" t="n">
         <v>45881</v>
       </c>
-      <c r="M4" t="n">
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="n">
         <v>0.8333333333333334</v>
       </c>
-      <c r="N4" t="n">
+      <c r="P4" t="n">
         <v>8.333333333333334</v>
       </c>
-      <c r="O4" t="n">
+      <c r="Q4" t="n">
         <v>0.4166666666666667</v>
       </c>
-      <c r="P4" t="n">
+      <c r="R4" t="n">
         <v>8.75</v>
       </c>
-      <c r="Q4" t="inlineStr">
+      <c r="S4" t="inlineStr">
         <is>
           <t>August 2025</t>
         </is>
@@ -736,25 +748,25 @@
       <c r="J5" t="n">
         <v>95000</v>
       </c>
-      <c r="K5" t="n">
-        <v>50000</v>
-      </c>
+      <c r="K5" t="inlineStr"/>
       <c r="L5" s="2" t="n">
         <v>45882</v>
       </c>
-      <c r="M5" t="n">
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="n">
         <v>1.166666666666667</v>
       </c>
-      <c r="N5" t="n">
+      <c r="P5" t="n">
         <v>5.833333333333334</v>
       </c>
-      <c r="O5" t="n">
+      <c r="Q5" t="n">
         <v>0.2916666666666667</v>
       </c>
-      <c r="P5" t="n">
+      <c r="R5" t="n">
         <v>6.125000000000001</v>
       </c>
-      <c r="Q5" t="inlineStr">
+      <c r="S5" t="inlineStr">
         <is>
           <t>August 2025</t>
         </is>
@@ -795,25 +807,25 @@
       <c r="J6" t="n">
         <v>98000</v>
       </c>
-      <c r="K6" t="n">
-        <v>890000</v>
-      </c>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" s="2" t="n">
         <v>45883</v>
       </c>
-      <c r="M6" t="n">
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="n">
         <v>2.266666666666667</v>
       </c>
-      <c r="N6" t="n">
+      <c r="P6" t="n">
         <v>15.86666666666667</v>
       </c>
-      <c r="O6" t="n">
+      <c r="Q6" t="n">
         <v>0.7933333333333334</v>
       </c>
-      <c r="P6" t="n">
+      <c r="R6" t="n">
         <v>16.66</v>
       </c>
-      <c r="Q6" t="inlineStr">
+      <c r="S6" t="inlineStr">
         <is>
           <t>August 2025</t>
         </is>
@@ -854,25 +866,25 @@
       <c r="J7" t="n">
         <v>78000</v>
       </c>
-      <c r="K7" t="n">
-        <v>1000000</v>
-      </c>
+      <c r="K7" t="inlineStr"/>
       <c r="L7" s="2" t="n">
         <v>45884</v>
       </c>
-      <c r="M7" t="n">
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="n">
         <v>1.6</v>
       </c>
-      <c r="N7" t="n">
+      <c r="P7" t="n">
         <v>16</v>
       </c>
-      <c r="O7" t="n">
+      <c r="Q7" t="n">
         <v>0.8</v>
       </c>
-      <c r="P7" t="n">
+      <c r="R7" t="n">
         <v>16.8</v>
       </c>
-      <c r="Q7" t="inlineStr">
+      <c r="S7" t="inlineStr">
         <is>
           <t>August 2025</t>
         </is>
@@ -913,25 +925,25 @@
       <c r="J8" t="n">
         <v>89000</v>
       </c>
-      <c r="K8" t="n">
-        <v>1200000</v>
-      </c>
+      <c r="K8" t="inlineStr"/>
       <c r="L8" s="2" t="n">
         <v>45885</v>
       </c>
-      <c r="M8" t="n">
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="n">
         <v>2</v>
       </c>
-      <c r="N8" t="n">
+      <c r="P8" t="n">
         <v>10</v>
       </c>
-      <c r="O8" t="n">
+      <c r="Q8" t="n">
         <v>0.5</v>
       </c>
-      <c r="P8" t="n">
+      <c r="R8" t="n">
         <v>10.5</v>
       </c>
-      <c r="Q8" t="inlineStr">
+      <c r="S8" t="inlineStr">
         <is>
           <t>August 2025</t>
         </is>
@@ -972,25 +984,25 @@
       <c r="J9" t="n">
         <v>90000</v>
       </c>
-      <c r="K9" t="n">
-        <v>950000</v>
-      </c>
+      <c r="K9" t="inlineStr"/>
       <c r="L9" s="2" t="n">
         <v>45886</v>
       </c>
-      <c r="M9" t="n">
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="n">
         <v>1.666666666666667</v>
       </c>
-      <c r="N9" t="n">
+      <c r="P9" t="n">
         <v>11.66666666666667</v>
       </c>
-      <c r="O9" t="n">
+      <c r="Q9" t="n">
         <v>0.5833333333333334</v>
       </c>
-      <c r="P9" t="n">
+      <c r="R9" t="n">
         <v>12.25</v>
       </c>
-      <c r="Q9" t="inlineStr">
+      <c r="S9" t="inlineStr">
         <is>
           <t>August 2025</t>
         </is>
@@ -1031,25 +1043,25 @@
       <c r="J10" t="n">
         <v>600000</v>
       </c>
-      <c r="K10" t="n">
-        <v>350000</v>
-      </c>
+      <c r="K10" t="inlineStr"/>
       <c r="L10" s="2" t="n">
         <v>45887</v>
       </c>
-      <c r="M10" t="n">
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="n">
         <v>1.333333333333333</v>
       </c>
-      <c r="N10" t="n">
+      <c r="P10" t="n">
         <v>13.33333333333333</v>
       </c>
-      <c r="O10" t="n">
+      <c r="Q10" t="n">
         <v>0.6666666666666666</v>
       </c>
-      <c r="P10" t="n">
+      <c r="R10" t="n">
         <v>14</v>
       </c>
-      <c r="Q10" t="inlineStr">
+      <c r="S10" t="inlineStr">
         <is>
           <t>August 2025</t>
         </is>
@@ -1090,25 +1102,25 @@
       <c r="J11" t="n">
         <v>600000</v>
       </c>
-      <c r="K11" t="n">
-        <v>350000</v>
-      </c>
+      <c r="K11" t="inlineStr"/>
       <c r="L11" s="2" t="n">
         <v>45888</v>
       </c>
-      <c r="M11" t="n">
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="n">
         <v>1.333333333333333</v>
       </c>
-      <c r="N11" t="n">
+      <c r="P11" t="n">
         <v>13.33333333333333</v>
       </c>
-      <c r="O11" t="n">
+      <c r="Q11" t="n">
         <v>0.6666666666666666</v>
       </c>
-      <c r="P11" t="n">
+      <c r="R11" t="n">
         <v>14</v>
       </c>
-      <c r="Q11" t="inlineStr">
+      <c r="S11" t="inlineStr">
         <is>
           <t>August 2025</t>
         </is>
@@ -1149,25 +1161,25 @@
       <c r="J12" t="n">
         <v>600000</v>
       </c>
-      <c r="K12" t="n">
-        <v>350000</v>
-      </c>
+      <c r="K12" t="inlineStr"/>
       <c r="L12" s="2" t="n">
         <v>45889</v>
       </c>
-      <c r="M12" t="n">
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="n">
         <v>1.333333333333333</v>
       </c>
-      <c r="N12" t="n">
+      <c r="P12" t="n">
         <v>13.33333333333333</v>
       </c>
-      <c r="O12" t="n">
+      <c r="Q12" t="n">
         <v>0.6666666666666666</v>
       </c>
-      <c r="P12" t="n">
+      <c r="R12" t="n">
         <v>14</v>
       </c>
-      <c r="Q12" t="inlineStr">
+      <c r="S12" t="inlineStr">
         <is>
           <t>August 2025</t>
         </is>
@@ -1208,25 +1220,25 @@
       <c r="J13" t="n">
         <v>600000</v>
       </c>
-      <c r="K13" t="n">
-        <v>350000</v>
-      </c>
+      <c r="K13" t="inlineStr"/>
       <c r="L13" s="2" t="n">
         <v>45890</v>
       </c>
-      <c r="M13" t="n">
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="n">
         <v>1.333333333333333</v>
       </c>
-      <c r="N13" t="n">
+      <c r="P13" t="n">
         <v>13.33333333333333</v>
       </c>
-      <c r="O13" t="n">
+      <c r="Q13" t="n">
         <v>0.6666666666666666</v>
       </c>
-      <c r="P13" t="n">
+      <c r="R13" t="n">
         <v>14</v>
       </c>
-      <c r="Q13" t="inlineStr">
+      <c r="S13" t="inlineStr">
         <is>
           <t>August 2025</t>
         </is>
@@ -1267,25 +1279,25 @@
       <c r="J14" t="n">
         <v>600000</v>
       </c>
-      <c r="K14" t="n">
-        <v>350000</v>
-      </c>
+      <c r="K14" t="inlineStr"/>
       <c r="L14" s="2" t="n">
         <v>45891</v>
       </c>
-      <c r="M14" t="n">
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr"/>
+      <c r="O14" t="n">
         <v>1.333333333333333</v>
       </c>
-      <c r="N14" t="n">
+      <c r="P14" t="n">
         <v>13.33333333333333</v>
       </c>
-      <c r="O14" t="n">
+      <c r="Q14" t="n">
         <v>0.6666666666666666</v>
       </c>
-      <c r="P14" t="n">
+      <c r="R14" t="n">
         <v>14</v>
       </c>
-      <c r="Q14" t="inlineStr">
+      <c r="S14" t="inlineStr">
         <is>
           <t>August 2025</t>
         </is>

</xml_diff>

<commit_message>
cifras de informe pdf corregido
</commit_message>
<xml_diff>
--- a/app/static/inventario_calculado.xlsx
+++ b/app/static/inventario_calculado.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S14"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -500,35 +500,25 @@
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 12</t>
+          <t>Demanda diaria</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 13</t>
+          <t>Stock mínimo</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Demanda diaria</t>
+          <t>Stock seguridad</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>Stock mínimo</t>
+          <t>Stock máximo</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>Stock seguridad</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>Stock máximo</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Mes</t>
         </is>
@@ -569,27 +559,25 @@
       <c r="J2" t="n">
         <v>800000</v>
       </c>
-      <c r="K2" t="inlineStr"/>
+      <c r="K2" t="n">
+        <v>900000</v>
+      </c>
       <c r="L2" s="2" t="n">
         <v>45879</v>
       </c>
-      <c r="M2" t="inlineStr"/>
+      <c r="M2" t="n">
+        <v>2</v>
+      </c>
       <c r="N2" t="n">
-        <v>2840000</v>
+        <v>10</v>
       </c>
       <c r="O2" t="n">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="P2" t="n">
-        <v>10</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="R2" t="n">
         <v>10.5</v>
       </c>
-      <c r="S2" t="inlineStr">
+      <c r="Q2" t="inlineStr">
         <is>
           <t>August 2025</t>
         </is>
@@ -630,25 +618,25 @@
       <c r="J3" t="n">
         <v>900000</v>
       </c>
-      <c r="K3" t="inlineStr"/>
+      <c r="K3" t="n">
+        <v>300000</v>
+      </c>
       <c r="L3" s="2" t="n">
         <v>45880</v>
       </c>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
+      <c r="M3" t="n">
+        <v>2.666666666666667</v>
+      </c>
+      <c r="N3" t="n">
+        <v>18.66666666666666</v>
+      </c>
       <c r="O3" t="n">
-        <v>2.666666666666667</v>
+        <v>0.9333333333333332</v>
       </c>
       <c r="P3" t="n">
-        <v>18.66666666666666</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>0.9333333333333332</v>
-      </c>
-      <c r="R3" t="n">
         <v>19.6</v>
       </c>
-      <c r="S3" t="inlineStr">
+      <c r="Q3" t="inlineStr">
         <is>
           <t>August 2025</t>
         </is>
@@ -689,25 +677,25 @@
       <c r="J4" t="n">
         <v>150000</v>
       </c>
-      <c r="K4" t="inlineStr"/>
+      <c r="K4" t="n">
+        <v>100000</v>
+      </c>
       <c r="L4" s="2" t="n">
         <v>45881</v>
       </c>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
+      <c r="M4" t="n">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="N4" t="n">
+        <v>8.333333333333334</v>
+      </c>
       <c r="O4" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.4166666666666667</v>
       </c>
       <c r="P4" t="n">
-        <v>8.333333333333334</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>0.4166666666666667</v>
-      </c>
-      <c r="R4" t="n">
         <v>8.75</v>
       </c>
-      <c r="S4" t="inlineStr">
+      <c r="Q4" t="inlineStr">
         <is>
           <t>August 2025</t>
         </is>
@@ -748,25 +736,25 @@
       <c r="J5" t="n">
         <v>95000</v>
       </c>
-      <c r="K5" t="inlineStr"/>
+      <c r="K5" t="n">
+        <v>50000</v>
+      </c>
       <c r="L5" s="2" t="n">
         <v>45882</v>
       </c>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
+      <c r="M5" t="n">
+        <v>1.166666666666667</v>
+      </c>
+      <c r="N5" t="n">
+        <v>5.833333333333334</v>
+      </c>
       <c r="O5" t="n">
-        <v>1.166666666666667</v>
+        <v>0.2916666666666667</v>
       </c>
       <c r="P5" t="n">
-        <v>5.833333333333334</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>0.2916666666666667</v>
-      </c>
-      <c r="R5" t="n">
         <v>6.125000000000001</v>
       </c>
-      <c r="S5" t="inlineStr">
+      <c r="Q5" t="inlineStr">
         <is>
           <t>August 2025</t>
         </is>
@@ -807,25 +795,25 @@
       <c r="J6" t="n">
         <v>98000</v>
       </c>
-      <c r="K6" t="inlineStr"/>
+      <c r="K6" t="n">
+        <v>890000</v>
+      </c>
       <c r="L6" s="2" t="n">
         <v>45883</v>
       </c>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
+      <c r="M6" t="n">
+        <v>2.266666666666667</v>
+      </c>
+      <c r="N6" t="n">
+        <v>15.86666666666667</v>
+      </c>
       <c r="O6" t="n">
-        <v>2.266666666666667</v>
+        <v>0.7933333333333334</v>
       </c>
       <c r="P6" t="n">
-        <v>15.86666666666667</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>0.7933333333333334</v>
-      </c>
-      <c r="R6" t="n">
         <v>16.66</v>
       </c>
-      <c r="S6" t="inlineStr">
+      <c r="Q6" t="inlineStr">
         <is>
           <t>August 2025</t>
         </is>
@@ -866,25 +854,25 @@
       <c r="J7" t="n">
         <v>78000</v>
       </c>
-      <c r="K7" t="inlineStr"/>
+      <c r="K7" t="n">
+        <v>1000000</v>
+      </c>
       <c r="L7" s="2" t="n">
         <v>45884</v>
       </c>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
+      <c r="M7" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="N7" t="n">
+        <v>16</v>
+      </c>
       <c r="O7" t="n">
-        <v>1.6</v>
+        <v>0.8</v>
       </c>
       <c r="P7" t="n">
-        <v>16</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="R7" t="n">
         <v>16.8</v>
       </c>
-      <c r="S7" t="inlineStr">
+      <c r="Q7" t="inlineStr">
         <is>
           <t>August 2025</t>
         </is>
@@ -925,25 +913,25 @@
       <c r="J8" t="n">
         <v>89000</v>
       </c>
-      <c r="K8" t="inlineStr"/>
+      <c r="K8" t="n">
+        <v>1200000</v>
+      </c>
       <c r="L8" s="2" t="n">
         <v>45885</v>
       </c>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
+      <c r="M8" t="n">
+        <v>2</v>
+      </c>
+      <c r="N8" t="n">
+        <v>10</v>
+      </c>
       <c r="O8" t="n">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="P8" t="n">
-        <v>10</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="R8" t="n">
         <v>10.5</v>
       </c>
-      <c r="S8" t="inlineStr">
+      <c r="Q8" t="inlineStr">
         <is>
           <t>August 2025</t>
         </is>
@@ -984,25 +972,25 @@
       <c r="J9" t="n">
         <v>90000</v>
       </c>
-      <c r="K9" t="inlineStr"/>
+      <c r="K9" t="n">
+        <v>950000</v>
+      </c>
       <c r="L9" s="2" t="n">
         <v>45886</v>
       </c>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
+      <c r="M9" t="n">
+        <v>1.666666666666667</v>
+      </c>
+      <c r="N9" t="n">
+        <v>11.66666666666667</v>
+      </c>
       <c r="O9" t="n">
-        <v>1.666666666666667</v>
+        <v>0.5833333333333334</v>
       </c>
       <c r="P9" t="n">
-        <v>11.66666666666667</v>
-      </c>
-      <c r="Q9" t="n">
-        <v>0.5833333333333334</v>
-      </c>
-      <c r="R9" t="n">
         <v>12.25</v>
       </c>
-      <c r="S9" t="inlineStr">
+      <c r="Q9" t="inlineStr">
         <is>
           <t>August 2025</t>
         </is>
@@ -1043,25 +1031,25 @@
       <c r="J10" t="n">
         <v>600000</v>
       </c>
-      <c r="K10" t="inlineStr"/>
+      <c r="K10" t="n">
+        <v>350000</v>
+      </c>
       <c r="L10" s="2" t="n">
         <v>45887</v>
       </c>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
+      <c r="M10" t="n">
+        <v>1.333333333333333</v>
+      </c>
+      <c r="N10" t="n">
+        <v>13.33333333333333</v>
+      </c>
       <c r="O10" t="n">
-        <v>1.333333333333333</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="P10" t="n">
-        <v>13.33333333333333</v>
-      </c>
-      <c r="Q10" t="n">
-        <v>0.6666666666666666</v>
-      </c>
-      <c r="R10" t="n">
         <v>14</v>
       </c>
-      <c r="S10" t="inlineStr">
+      <c r="Q10" t="inlineStr">
         <is>
           <t>August 2025</t>
         </is>
@@ -1102,25 +1090,25 @@
       <c r="J11" t="n">
         <v>600000</v>
       </c>
-      <c r="K11" t="inlineStr"/>
+      <c r="K11" t="n">
+        <v>350000</v>
+      </c>
       <c r="L11" s="2" t="n">
         <v>45888</v>
       </c>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
+      <c r="M11" t="n">
+        <v>1.333333333333333</v>
+      </c>
+      <c r="N11" t="n">
+        <v>13.33333333333333</v>
+      </c>
       <c r="O11" t="n">
-        <v>1.333333333333333</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="P11" t="n">
-        <v>13.33333333333333</v>
-      </c>
-      <c r="Q11" t="n">
-        <v>0.6666666666666666</v>
-      </c>
-      <c r="R11" t="n">
         <v>14</v>
       </c>
-      <c r="S11" t="inlineStr">
+      <c r="Q11" t="inlineStr">
         <is>
           <t>August 2025</t>
         </is>
@@ -1161,25 +1149,25 @@
       <c r="J12" t="n">
         <v>600000</v>
       </c>
-      <c r="K12" t="inlineStr"/>
+      <c r="K12" t="n">
+        <v>350000</v>
+      </c>
       <c r="L12" s="2" t="n">
         <v>45889</v>
       </c>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
+      <c r="M12" t="n">
+        <v>1.333333333333333</v>
+      </c>
+      <c r="N12" t="n">
+        <v>13.33333333333333</v>
+      </c>
       <c r="O12" t="n">
-        <v>1.333333333333333</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="P12" t="n">
-        <v>13.33333333333333</v>
-      </c>
-      <c r="Q12" t="n">
-        <v>0.6666666666666666</v>
-      </c>
-      <c r="R12" t="n">
         <v>14</v>
       </c>
-      <c r="S12" t="inlineStr">
+      <c r="Q12" t="inlineStr">
         <is>
           <t>August 2025</t>
         </is>
@@ -1220,25 +1208,25 @@
       <c r="J13" t="n">
         <v>600000</v>
       </c>
-      <c r="K13" t="inlineStr"/>
+      <c r="K13" t="n">
+        <v>350000</v>
+      </c>
       <c r="L13" s="2" t="n">
         <v>45890</v>
       </c>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr"/>
+      <c r="M13" t="n">
+        <v>1.333333333333333</v>
+      </c>
+      <c r="N13" t="n">
+        <v>13.33333333333333</v>
+      </c>
       <c r="O13" t="n">
-        <v>1.333333333333333</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="P13" t="n">
-        <v>13.33333333333333</v>
-      </c>
-      <c r="Q13" t="n">
-        <v>0.6666666666666666</v>
-      </c>
-      <c r="R13" t="n">
         <v>14</v>
       </c>
-      <c r="S13" t="inlineStr">
+      <c r="Q13" t="inlineStr">
         <is>
           <t>August 2025</t>
         </is>
@@ -1279,25 +1267,25 @@
       <c r="J14" t="n">
         <v>600000</v>
       </c>
-      <c r="K14" t="inlineStr"/>
+      <c r="K14" t="n">
+        <v>350000</v>
+      </c>
       <c r="L14" s="2" t="n">
         <v>45891</v>
       </c>
-      <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr"/>
+      <c r="M14" t="n">
+        <v>1.333333333333333</v>
+      </c>
+      <c r="N14" t="n">
+        <v>13.33333333333333</v>
+      </c>
       <c r="O14" t="n">
-        <v>1.333333333333333</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="P14" t="n">
-        <v>13.33333333333333</v>
-      </c>
-      <c r="Q14" t="n">
-        <v>0.6666666666666666</v>
-      </c>
-      <c r="R14" t="n">
         <v>14</v>
       </c>
-      <c r="S14" t="inlineStr">
+      <c r="Q14" t="inlineStr">
         <is>
           <t>August 2025</t>
         </is>

</xml_diff>